<commit_message>
fix: chatbot remember initial prompt
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\SKRIPSI\Rekomendasi-Notulensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85372E37-4145-434F-9337-CC5BDD112AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F142A13D-22FF-4BDF-9EB2-AEACEE9A8443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2925,20 +2925,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12874,7 +12874,7 @@
   <dimension ref="B1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -13107,10 +13107,10 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>893</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>894</v>
       </c>
     </row>
@@ -13121,10 +13121,10 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="23" t="s">
         <v>895</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="21" t="s">
         <v>898</v>
       </c>
     </row>
@@ -13135,8 +13135,8 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="24" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="21" t="s">
         <v>903</v>
       </c>
     </row>
@@ -13147,10 +13147,10 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="23" t="s">
         <v>896</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="21" t="s">
         <v>899</v>
       </c>
     </row>
@@ -13161,8 +13161,8 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="24" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="21" t="s">
         <v>902</v>
       </c>
     </row>
@@ -13173,10 +13173,10 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="24" t="s">
         <v>897</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="21" t="s">
         <v>900</v>
       </c>
     </row>
@@ -13187,8 +13187,8 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="24" t="s">
+      <c r="E10" s="24"/>
+      <c r="F10" s="21" t="s">
         <v>901</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Updated app.py to add description and instructions, modified table display, and initialized session state variables;
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\SKRIPSI\Rekomendasi-Notulensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F142A13D-22FF-4BDF-9EB2-AEACEE9A8443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48046F4C-C5FD-4EBA-AFFE-551D927341AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="936">
   <si>
     <t>Notulen</t>
   </si>
@@ -2751,6 +2751,99 @@
   </si>
   <si>
     <t>Beri nomor tabel di atas tabel</t>
+  </si>
+  <si>
+    <t>Agatha B</t>
+  </si>
+  <si>
+    <t>Windy</t>
+  </si>
+  <si>
+    <t>Alvina</t>
+  </si>
+  <si>
+    <t>Annisa</t>
+  </si>
+  <si>
+    <t>Apin</t>
+  </si>
+  <si>
+    <t>Elsa</t>
+  </si>
+  <si>
+    <t>Paman</t>
+  </si>
+  <si>
+    <t>Hafidh</t>
+  </si>
+  <si>
+    <t>Ibad</t>
+  </si>
+  <si>
+    <t>Jahfal</t>
+  </si>
+  <si>
+    <t>Leli</t>
+  </si>
+  <si>
+    <t>Ramzi</t>
+  </si>
+  <si>
+    <t>Satria</t>
+  </si>
+  <si>
+    <t>Selena</t>
+  </si>
+  <si>
+    <t>Vannesa</t>
+  </si>
+  <si>
+    <t>Bara</t>
+  </si>
+  <si>
+    <t>Alam</t>
+  </si>
+  <si>
+    <t>Nanggala</t>
+  </si>
+  <si>
+    <t>Vio</t>
+  </si>
+  <si>
+    <t>Fajar</t>
+  </si>
+  <si>
+    <t>Yogi</t>
+  </si>
+  <si>
+    <t>Krisi</t>
+  </si>
+  <si>
+    <t>Rafli</t>
+  </si>
+  <si>
+    <t>Rafi</t>
+  </si>
+  <si>
+    <t>Gopal</t>
+  </si>
+  <si>
+    <t>Elroy</t>
+  </si>
+  <si>
+    <t>Janu</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Aryanti</t>
+  </si>
+  <si>
+    <t>Julpi</t>
+  </si>
+  <si>
+    <t>Aldi</t>
   </si>
 </sst>
 </file>
@@ -2833,7 +2926,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2843,6 +2936,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2884,7 +2983,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2931,6 +3030,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12874,7 +12975,7 @@
   <dimension ref="B1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -13075,15 +13176,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA58419B-EB0A-46B3-BB9B-601F39D6F4A5}">
-  <dimension ref="B3:F18"/>
+  <dimension ref="B3:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="87.85546875" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.42578125" customWidth="1"/>
   </cols>
@@ -13095,10 +13196,10 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="22"/>
+      <c r="E3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
@@ -13121,7 +13222,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="25" t="s">
         <v>895</v>
       </c>
       <c r="F5" s="21" t="s">
@@ -13135,7 +13236,7 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="21" t="s">
         <v>903</v>
       </c>
@@ -13147,7 +13248,7 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="25" t="s">
         <v>896</v>
       </c>
       <c r="F7" s="21" t="s">
@@ -13161,7 +13262,7 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="21" t="s">
         <v>902</v>
       </c>
@@ -13173,7 +13274,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="26" t="s">
         <v>897</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -13187,7 +13288,7 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="21" t="s">
         <v>901</v>
       </c>
@@ -13254,6 +13355,161 @@
       </c>
       <c r="C18">
         <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="22" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="22" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="22" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="22" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="22" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="22" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="22" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="22" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="22" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="22" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="22" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="22" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="22" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="22" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="22" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="22" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="22" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="22" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="22" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="22" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="22" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="23" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="23" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="23" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="23" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="23" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="22" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="23" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="23" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="23" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="22" t="s">
+        <v>935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: parafrase initial msg
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\SKRIPSI\Rekomendasi-Notulensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC909BD-C1E7-4A1A-806E-FE395EDD2C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6EA5C6-4BAA-466D-99BD-A065C3FB6366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="1004">
   <si>
     <t>Notulen</t>
   </si>
@@ -3032,6 +3032,24 @@
   </si>
   <si>
     <t>Dimas</t>
+  </si>
+  <si>
+    <t>Vitor</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>RBF</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>Akurasi</t>
   </si>
 </sst>
 </file>
@@ -3041,7 +3059,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3163,6 +3181,12 @@
       <name val="Book Antiqua"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3228,11 +3252,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3343,7 +3368,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3356,11 +3389,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{A2072F88-2B3B-45F5-9993-92A3319DEB14}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3640,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M868"/>
   <sheetViews>
-    <sheetView topLeftCell="C75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89:G94"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3651,8 +3684,8 @@
     <col min="3" max="3" width="8.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="10" width="15.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="51" style="6" customWidth="1"/>
@@ -3873,7 +3906,9 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="8"/>
+      <c r="L9" s="26" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="12">
@@ -3896,7 +3931,9 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="8"/>
+      <c r="L10" s="20" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="12">
@@ -3919,7 +3956,9 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="8"/>
+      <c r="L11" s="20" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="12">
@@ -3943,7 +3982,9 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="8"/>
+      <c r="L12" s="20" t="s">
+        <v>945</v>
+      </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="12">
@@ -3961,7 +4002,9 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="8"/>
+      <c r="L13" s="20" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="12">
@@ -3982,7 +4025,9 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="8"/>
+      <c r="L14" s="20" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="12">
@@ -4883,7 +4928,7 @@
       <c r="C62" s="14">
         <v>2</v>
       </c>
-      <c r="E62" s="49" t="s">
+      <c r="E62" s="55" t="s">
         <v>981</v>
       </c>
       <c r="F62" s="46">
@@ -4903,7 +4948,7 @@
       <c r="C63" s="14">
         <v>1</v>
       </c>
-      <c r="E63" s="49"/>
+      <c r="E63" s="55"/>
       <c r="F63" s="46">
         <v>0.2</v>
       </c>
@@ -4921,7 +4966,7 @@
       <c r="C64" s="14">
         <v>3</v>
       </c>
-      <c r="E64" s="49"/>
+      <c r="E64" s="55"/>
       <c r="F64" s="46">
         <v>0.3</v>
       </c>
@@ -4939,7 +4984,7 @@
       <c r="C65" s="14">
         <v>2</v>
       </c>
-      <c r="E65" s="49"/>
+      <c r="E65" s="55"/>
       <c r="F65" s="46">
         <v>0.4</v>
       </c>
@@ -4957,7 +5002,7 @@
       <c r="C66" s="14">
         <v>1</v>
       </c>
-      <c r="E66" s="49"/>
+      <c r="E66" s="55"/>
       <c r="F66" s="46">
         <v>0.5</v>
       </c>
@@ -4975,7 +5020,7 @@
       <c r="C67" s="14">
         <v>2</v>
       </c>
-      <c r="E67" s="49" t="s">
+      <c r="E67" s="55" t="s">
         <v>982</v>
       </c>
       <c r="F67" s="46">
@@ -4995,7 +5040,7 @@
       <c r="C68" s="14">
         <v>3</v>
       </c>
-      <c r="E68" s="49"/>
+      <c r="E68" s="55"/>
       <c r="F68" s="46">
         <v>0.2</v>
       </c>
@@ -5013,7 +5058,7 @@
       <c r="C69" s="14">
         <v>1</v>
       </c>
-      <c r="E69" s="49"/>
+      <c r="E69" s="55"/>
       <c r="F69" s="46">
         <v>0.3</v>
       </c>
@@ -5031,7 +5076,7 @@
       <c r="C70" s="14">
         <v>3</v>
       </c>
-      <c r="E70" s="49"/>
+      <c r="E70" s="55"/>
       <c r="F70" s="46">
         <v>0.4</v>
       </c>
@@ -5049,7 +5094,7 @@
       <c r="C71" s="14">
         <v>2</v>
       </c>
-      <c r="E71" s="49"/>
+      <c r="E71" s="55"/>
       <c r="F71" s="46">
         <v>0.5</v>
       </c>
@@ -5067,7 +5112,7 @@
       <c r="C72" s="14">
         <v>1</v>
       </c>
-      <c r="E72" s="49" t="s">
+      <c r="E72" s="55" t="s">
         <v>983</v>
       </c>
       <c r="F72" s="46">
@@ -5087,7 +5132,7 @@
       <c r="C73" s="14">
         <v>3</v>
       </c>
-      <c r="E73" s="49"/>
+      <c r="E73" s="55"/>
       <c r="F73" s="46">
         <v>0.2</v>
       </c>
@@ -5105,7 +5150,7 @@
       <c r="C74" s="14">
         <v>2</v>
       </c>
-      <c r="E74" s="49"/>
+      <c r="E74" s="55"/>
       <c r="F74" s="46">
         <v>0.3</v>
       </c>
@@ -5123,7 +5168,7 @@
       <c r="C75" s="14">
         <v>1</v>
       </c>
-      <c r="E75" s="49"/>
+      <c r="E75" s="55"/>
       <c r="F75" s="46">
         <v>0.4</v>
       </c>
@@ -5141,7 +5186,7 @@
       <c r="C76" s="14">
         <v>2</v>
       </c>
-      <c r="E76" s="49"/>
+      <c r="E76" s="55"/>
       <c r="F76" s="46">
         <v>0.5</v>
       </c>
@@ -5159,7 +5204,7 @@
       <c r="C77" s="14">
         <v>1</v>
       </c>
-      <c r="E77" s="49" t="s">
+      <c r="E77" s="55" t="s">
         <v>984</v>
       </c>
       <c r="F77" s="46">
@@ -5179,7 +5224,7 @@
       <c r="C78" s="14">
         <v>3</v>
       </c>
-      <c r="E78" s="49"/>
+      <c r="E78" s="55"/>
       <c r="F78" s="46">
         <v>0.2</v>
       </c>
@@ -5197,7 +5242,7 @@
       <c r="C79" s="14">
         <v>1</v>
       </c>
-      <c r="E79" s="49"/>
+      <c r="E79" s="55"/>
       <c r="F79" s="46">
         <v>0.3</v>
       </c>
@@ -5215,7 +5260,7 @@
       <c r="C80" s="14">
         <v>2</v>
       </c>
-      <c r="E80" s="49"/>
+      <c r="E80" s="55"/>
       <c r="F80" s="46">
         <v>0.4</v>
       </c>
@@ -5233,7 +5278,7 @@
       <c r="C81" s="14">
         <v>3</v>
       </c>
-      <c r="E81" s="49"/>
+      <c r="E81" s="55"/>
       <c r="F81" s="46">
         <v>0.5</v>
       </c>
@@ -5251,7 +5296,7 @@
       <c r="C82" s="14">
         <v>1</v>
       </c>
-      <c r="E82" s="49" t="s">
+      <c r="E82" s="55" t="s">
         <v>985</v>
       </c>
       <c r="F82" s="46">
@@ -5271,7 +5316,7 @@
       <c r="C83" s="14">
         <v>2</v>
       </c>
-      <c r="E83" s="49"/>
+      <c r="E83" s="55"/>
       <c r="F83" s="46">
         <v>0.2</v>
       </c>
@@ -5289,7 +5334,7 @@
       <c r="C84" s="14">
         <v>3</v>
       </c>
-      <c r="E84" s="49"/>
+      <c r="E84" s="55"/>
       <c r="F84" s="46">
         <v>0.3</v>
       </c>
@@ -5307,7 +5352,7 @@
       <c r="C85" s="14">
         <v>1</v>
       </c>
-      <c r="E85" s="49"/>
+      <c r="E85" s="55"/>
       <c r="F85" s="46">
         <v>0.4</v>
       </c>
@@ -5325,7 +5370,7 @@
       <c r="C86" s="14">
         <v>2</v>
       </c>
-      <c r="E86" s="49"/>
+      <c r="E86" s="55"/>
       <c r="F86" s="46">
         <v>0.5</v>
       </c>
@@ -5502,7 +5547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:10">
       <c r="A97" s="12">
         <v>96</v>
       </c>
@@ -5512,8 +5557,26 @@
       <c r="C97" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="E97" s="53" t="s">
+        <v>999</v>
+      </c>
+      <c r="F97" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="G97" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="H97" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="I97" s="54">
+        <v>0.4</v>
+      </c>
+      <c r="J97" s="54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="12">
         <v>97</v>
       </c>
@@ -5523,8 +5586,26 @@
       <c r="C98" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="E98" s="46" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F98" s="52">
+        <v>0.68</v>
+      </c>
+      <c r="G98" s="52">
+        <v>0.67</v>
+      </c>
+      <c r="H98" s="52">
+        <v>0.66</v>
+      </c>
+      <c r="I98" s="52">
+        <v>0.64</v>
+      </c>
+      <c r="J98" s="52">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="12">
         <v>98</v>
       </c>
@@ -5534,8 +5615,26 @@
       <c r="C99" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="E99" s="46" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F99" s="52">
+        <v>0.82</v>
+      </c>
+      <c r="G99" s="52">
+        <v>0.79</v>
+      </c>
+      <c r="H99" s="52">
+        <v>0.76</v>
+      </c>
+      <c r="I99" s="52">
+        <v>0.72</v>
+      </c>
+      <c r="J99" s="52">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="12">
         <v>99</v>
       </c>
@@ -5546,7 +5645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:10">
       <c r="A101" s="12">
         <v>100</v>
       </c>
@@ -5557,7 +5656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:10">
       <c r="A102" s="12">
         <v>101</v>
       </c>
@@ -5568,7 +5667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:10">
       <c r="A103" s="12">
         <v>102</v>
       </c>
@@ -5578,8 +5677,26 @@
       <c r="C103" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="E103" s="20" t="s">
+        <v>966</v>
+      </c>
+      <c r="F103" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G103" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="H103" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="I103" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="J103" s="20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="12">
         <v>103</v>
       </c>
@@ -5589,8 +5706,26 @@
       <c r="C104" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="E104" s="20" t="s">
+        <v>999</v>
+      </c>
+      <c r="F104" s="20" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G104" s="20" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H104" s="20" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I104" s="20" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J104" s="20" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="12">
         <v>104</v>
       </c>
@@ -5600,8 +5735,26 @@
       <c r="C105" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="E105" s="20" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F105" s="52">
+        <v>0.82</v>
+      </c>
+      <c r="G105" s="52">
+        <v>0.79</v>
+      </c>
+      <c r="H105" s="52">
+        <v>0.75</v>
+      </c>
+      <c r="I105" s="52">
+        <v>0.71</v>
+      </c>
+      <c r="J105" s="52">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="12">
         <v>105</v>
       </c>
@@ -5612,7 +5765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:10">
       <c r="A107" s="12">
         <v>106</v>
       </c>
@@ -5623,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:10">
       <c r="A108" s="12">
         <v>107</v>
       </c>
@@ -5634,7 +5787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:10">
       <c r="A109" s="12">
         <v>108</v>
       </c>
@@ -5645,7 +5798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:10">
       <c r="A110" s="12">
         <v>109</v>
       </c>
@@ -5656,7 +5809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:10">
       <c r="A111" s="12">
         <v>110</v>
       </c>
@@ -5667,7 +5820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:10">
       <c r="A112" s="12">
         <v>111</v>
       </c>
@@ -14213,10 +14366,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA58419B-EB0A-46B3-BB9B-601F39D6F4A5}">
-  <dimension ref="A3:F62"/>
+  <dimension ref="A3:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14234,10 +14387,10 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="50"/>
+      <c r="E3" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
@@ -14260,7 +14413,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="57" t="s">
         <v>895</v>
       </c>
       <c r="F5" s="19" t="s">
@@ -14274,7 +14427,7 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="E6" s="51"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="19" t="s">
         <v>903</v>
       </c>
@@ -14286,7 +14439,7 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="57" t="s">
         <v>896</v>
       </c>
       <c r="F7" s="19" t="s">
@@ -14300,7 +14453,7 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="E8" s="51"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="19" t="s">
         <v>902</v>
       </c>
@@ -14312,7 +14465,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="58" t="s">
         <v>897</v>
       </c>
       <c r="F9" s="19" t="s">
@@ -14326,7 +14479,7 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="E10" s="52"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="19" t="s">
         <v>901</v>
       </c>
@@ -14396,7 +14549,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23">
+      <c r="A23" s="20">
         <v>1</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -14404,7 +14557,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24">
+      <c r="A24" s="20">
         <v>2</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -14412,7 +14565,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25">
+      <c r="A25" s="20">
         <v>3</v>
       </c>
       <c r="B25" s="21" t="s">
@@ -14420,7 +14573,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26">
+      <c r="A26" s="20">
         <v>4</v>
       </c>
       <c r="B26" s="21" t="s">
@@ -14428,15 +14581,15 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27">
+      <c r="A27" s="20">
         <v>5</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28">
+      <c r="A28" s="20">
         <v>6</v>
       </c>
       <c r="B28" s="21" t="s">
@@ -14444,7 +14597,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29">
+      <c r="A29" s="20">
         <v>7</v>
       </c>
       <c r="B29" s="21" t="s">
@@ -14452,7 +14605,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30">
+      <c r="A30" s="20">
         <v>8</v>
       </c>
       <c r="B30" s="21" t="s">
@@ -14460,7 +14613,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31">
+      <c r="A31" s="20">
         <v>9</v>
       </c>
       <c r="B31" s="21" t="s">
@@ -14468,7 +14621,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32">
+      <c r="A32" s="20">
         <v>10</v>
       </c>
       <c r="B32" s="21" t="s">
@@ -14476,47 +14629,47 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33">
+      <c r="A33" s="20">
         <v>11</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="48" t="s">
         <v>914</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34">
+      <c r="A34" s="20">
         <v>12</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>915</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35">
+      <c r="A35" s="20">
         <v>13</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36">
+      <c r="A36" s="20">
         <v>14</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="49" t="s">
         <v>917</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37">
+      <c r="A37" s="20">
         <v>15</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>918</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38">
+      <c r="A38" s="20">
         <v>16</v>
       </c>
       <c r="B38" s="20" t="s">
@@ -14524,7 +14677,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39">
+      <c r="A39" s="20">
         <v>17</v>
       </c>
       <c r="B39" s="20" t="s">
@@ -14532,7 +14685,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40">
+      <c r="A40" s="20">
         <v>18</v>
       </c>
       <c r="B40" s="20" t="s">
@@ -14540,7 +14693,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41">
+      <c r="A41" s="20">
         <v>19</v>
       </c>
       <c r="B41" s="20" t="s">
@@ -14548,7 +14701,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42">
+      <c r="A42" s="20">
         <v>20</v>
       </c>
       <c r="B42" s="20" t="s">
@@ -14556,7 +14709,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43">
+      <c r="A43" s="20">
         <v>21</v>
       </c>
       <c r="B43" s="20" t="s">
@@ -14564,7 +14717,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44">
+      <c r="A44" s="20">
         <v>22</v>
       </c>
       <c r="B44" s="21" t="s">
@@ -14572,7 +14725,7 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45">
+      <c r="A45" s="20">
         <v>23</v>
       </c>
       <c r="B45" s="21" t="s">
@@ -14580,7 +14733,7 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46">
+      <c r="A46" s="20">
         <v>24</v>
       </c>
       <c r="B46" s="21" t="s">
@@ -14588,7 +14741,7 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47">
+      <c r="A47" s="20">
         <v>25</v>
       </c>
       <c r="B47" s="21" t="s">
@@ -14596,7 +14749,7 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48">
+      <c r="A48" s="20">
         <v>26</v>
       </c>
       <c r="B48" s="21" t="s">
@@ -14604,7 +14757,7 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49">
+      <c r="A49" s="20">
         <v>27</v>
       </c>
       <c r="B49" s="21" t="s">
@@ -14612,7 +14765,7 @@
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50">
+      <c r="A50" s="20">
         <v>28</v>
       </c>
       <c r="B50" s="21" t="s">
@@ -14620,7 +14773,7 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51">
+      <c r="A51" s="20">
         <v>29</v>
       </c>
       <c r="B51" s="21" t="s">
@@ -14628,7 +14781,7 @@
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52">
+      <c r="A52" s="20">
         <v>30</v>
       </c>
       <c r="B52" s="21" t="s">
@@ -14636,7 +14789,7 @@
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53">
+      <c r="A53" s="20">
         <v>31</v>
       </c>
       <c r="B53" s="20" t="s">
@@ -14644,7 +14797,7 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54">
+      <c r="A54" s="20">
         <v>32</v>
       </c>
       <c r="B54" s="21" t="s">
@@ -14652,7 +14805,7 @@
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55">
+      <c r="A55" s="20">
         <v>33</v>
       </c>
       <c r="B55" s="21" t="s">
@@ -14660,7 +14813,7 @@
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56">
+      <c r="A56" s="20">
         <v>34</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -14668,7 +14821,7 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57">
+      <c r="A57" s="20">
         <v>35</v>
       </c>
       <c r="B57" s="21" t="s">
@@ -14676,15 +14829,15 @@
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58">
+      <c r="A58" s="20">
         <v>36</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="21" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59">
+      <c r="A59" s="20">
         <v>37</v>
       </c>
       <c r="B59" s="21" t="s">
@@ -14692,7 +14845,7 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60">
+      <c r="A60" s="20">
         <v>38</v>
       </c>
       <c r="B60" s="21" t="s">
@@ -14700,7 +14853,7 @@
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61">
+      <c r="A61" s="20">
         <v>39</v>
       </c>
       <c r="B61" s="21" t="s">
@@ -14708,12 +14861,80 @@
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62">
+      <c r="A62" s="20">
         <v>40</v>
       </c>
-      <c r="B62" s="48" t="s">
+      <c r="B62" s="21" t="s">
         <v>997</v>
       </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="20">
+        <v>41</v>
+      </c>
+      <c r="B63" s="50" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="20">
+        <v>42</v>
+      </c>
+      <c r="B64" s="51"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="20">
+        <v>43</v>
+      </c>
+      <c r="B65" s="51"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="20">
+        <v>44</v>
+      </c>
+      <c r="B66" s="51"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="20">
+        <v>45</v>
+      </c>
+      <c r="B67" s="51"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="20">
+        <v>46</v>
+      </c>
+      <c r="B68" s="51"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="20">
+        <v>47</v>
+      </c>
+      <c r="B69" s="51"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="20">
+        <v>48</v>
+      </c>
+      <c r="B70" s="51"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="20">
+        <v>49</v>
+      </c>
+      <c r="B71" s="51"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="20">
+        <v>50</v>
+      </c>
+      <c r="B72" s="51"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="20">
+        <v>51</v>
+      </c>
+      <c r="B73" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>